<commit_message>
minimum spanning tree by kruskal method and activity selection problem
</commit_message>
<xml_diff>
--- a/graphs/graphs_concepts.xlsx
+++ b/graphs/graphs_concepts.xlsx
@@ -762,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF32" sqref="AF32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>